<commit_message>
Merge of fluvial into stable
</commit_message>
<xml_diff>
--- a/src/test/resources/bulk/bad_enum_value.xlsx
+++ b/src/test/resources/bulk/bad_enum_value.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="100" windowWidth="22040" windowHeight="12340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>filename</t>
   </si>
@@ -38,9 +38,6 @@
     <t>isbn</t>
   </si>
   <si>
-    <t>numberOfPages</t>
-  </si>
-  <si>
     <t>test1.pdf</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
   </si>
   <si>
     <t>1234-5312</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
   <si>
     <t>documentType</t>
@@ -425,15 +419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,64 +444,55 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>18</v>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2">
-        <v>1234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more bulk upload fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/bulk/bad_enum_value.xlsx
+++ b/src/test/resources/bulk/bad_enum_value.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16520"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>filename</t>
   </si>
@@ -81,16 +81,26 @@
   </si>
   <si>
     <t>BAD</t>
+  </si>
+  <si>
+    <t>Date Created (Year)*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,8 +126,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,79 +430,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Merge with dev branch (in situ)
</commit_message>
<xml_diff>
--- a/src/test/resources/bulk/bad_enum_value.xlsx
+++ b/src/test/resources/bulk/bad_enum_value.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16520"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>filename</t>
   </si>
@@ -81,16 +81,26 @@
   </si>
   <si>
     <t>BAD</t>
+  </si>
+  <si>
+    <t>Date Created (Year)*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,8 +126,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,79 +430,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>